<commit_message>
Added Fund Unit upload
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_units.xlsx
+++ b/public/sample_uploads/fund_units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE7A3C6-17B2-48FC-A604-C99862D31E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDE0A83-4547-4670-B4E2-173D51F076E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>Unit Type *</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Macro Fund</t>
   </si>
   <si>
-    <t>Capital Call 1695461797.3671792</t>
-  </si>
-  <si>
     <t>Series C</t>
   </si>
   <si>
@@ -76,25 +73,25 @@
   </si>
   <si>
     <t>Upload</t>
+  </si>
+  <si>
+    <t>Call 1</t>
+  </si>
+  <si>
+    <t>Call 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="5"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,9 +114,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -404,7 +400,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -459,11 +455,11 @@
       <c r="B2">
         <v>45742046</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -474,14 +470,14 @@
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>44562</v>
       </c>
       <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
@@ -491,11 +487,11 @@
       <c r="B3">
         <v>51694724</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
       </c>
       <c r="E3">
         <v>20</v>
@@ -506,14 +502,14 @@
       <c r="G3">
         <v>10</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>44562</v>
       </c>
       <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
         <v>15</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
@@ -523,11 +519,11 @@
       <c r="B4">
         <v>74056403</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
+      <c r="C4" t="s">
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -538,14 +534,14 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>44562</v>
       </c>
       <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
         <v>15</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
@@ -555,11 +551,11 @@
       <c r="B5">
         <v>89972901</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
+      <c r="C5" t="s">
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>40</v>
@@ -570,14 +566,14 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>44562</v>
       </c>
       <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
         <v>15</v>
-      </c>
-      <c r="J5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
@@ -587,11 +583,11 @@
       <c r="B6">
         <v>99305538</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
+      <c r="C6" t="s">
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6">
         <v>50</v>
@@ -602,14 +598,14 @@
       <c r="G6">
         <v>5</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>44562</v>
       </c>
       <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
         <v>15</v>
-      </c>
-      <c r="J6" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added check for correct unit type while importing fund units
</commit_message>
<xml_diff>
--- a/public/sample_uploads/fund_units.xlsx
+++ b/public/sample_uploads/fund_units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAB0F2A-BECE-4801-8698-F7CC1E01E61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE775DE-8AD0-44BF-9E30-62CE8B91F253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="17">
   <si>
     <t>Unit Type *</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Update Only *</t>
-  </si>
-  <si>
-    <t>Series C</t>
   </si>
   <si>
     <t>Series A</t>
@@ -134,11 +131,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +425,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D7" sqref="D7:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -450,7 +449,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -476,15 +475,15 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2">
@@ -500,23 +499,23 @@
         <v>44562</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E3">
@@ -532,23 +531,23 @@
         <v>44562</v>
       </c>
       <c r="I3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E4">
@@ -564,23 +563,23 @@
         <v>44562</v>
       </c>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E5">
@@ -596,24 +595,24 @@
         <v>44562</v>
       </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E6">
         <v>50</v>
@@ -628,23 +627,23 @@
         <v>44562</v>
       </c>
       <c r="I6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E7">
@@ -660,23 +659,23 @@
         <v>44927</v>
       </c>
       <c r="I7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E8">
@@ -692,23 +691,23 @@
         <v>44927</v>
       </c>
       <c r="I8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E9">
@@ -724,23 +723,23 @@
         <v>44927</v>
       </c>
       <c r="I9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E10">
@@ -756,24 +755,24 @@
         <v>44927</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="E11">
         <v>-25</v>
@@ -788,10 +787,10 @@
         <v>44927</v>
       </c>
       <c r="I11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>